<commit_message>
All Modules with initial code
</commit_message>
<xml_diff>
--- a/src/test/resources/exceldata/logindata.xlsx
+++ b/src/test/resources/exceldata/logindata.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Seema\Eclipse\Gitcode\dsalgo\src\test\resources\exceldata\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B6F45F65-F414-4D3A-A975-013827CBE0A0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4A7D3013-A54E-40F4-A072-7A711182AB49}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-20910" yWindow="-1770" windowWidth="21600" windowHeight="11145" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -111,12 +111,13 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
@@ -401,7 +402,7 @@
   <dimension ref="A1:C6"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C1" sqref="C1"/>
+      <selection activeCell="B5" sqref="B5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -458,7 +459,7 @@
       <c r="A5" t="s">
         <v>4</v>
       </c>
-      <c r="B5" t="s">
+      <c r="B5" s="3" t="s">
         <v>5</v>
       </c>
       <c r="C5" s="2" t="s">

</xml_diff>